<commit_message>
fast api implementation to consume agent response via api
</commit_message>
<xml_diff>
--- a/TestCases/test_case.xlsx
+++ b/TestCases/test_case.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Verify Email and Password Input Fields</t>
+          <t>Verify Email and Password Fields Display</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -467,19 +467,19 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify the presence of an input field labeled 'Email'.</t>
+          <t>Verify that two text fields are present: one labeled 'Email' and one labeled 'Password'.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>An input field labeled 'Email' is displayed.</t>
+          <t>Two text fields with the labels 'Email' and 'Password' are displayed.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Verify Password Input Field Masking</t>
+          <t>Verify Password Field Masking</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -493,19 +493,19 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hover over the 'Password' input field.</t>
+          <t>Enter text into the 'Password' field.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Entered characters in the 'Password' field are masked.</t>
+          <t>The entered characters in the 'Password' field are masked, not visible to the user.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Validate Empty Email Submission</t>
+          <t>Successful Login with Valid Credentials</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -519,7 +519,7 @@
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Enter an empty email address in the 'Email' field.</t>
+          <t>Enter valid email and password into the respective fields.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -533,14 +533,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>An error message is displayed indicating an empty email field is required.</t>
+          <t>The user is successfully redirected to the dashboard.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Validate Empty Password Submission</t>
+          <t>Successful Login with Mixed Case Credentials</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -554,7 +554,7 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Enter a valid email address in the 'Email' field.</t>
+          <t>Enter valid email and password with mixed case characters into the respective fields.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -563,33 +563,33 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Leave the 'Password' field empty.</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>Click the 'Login' button.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The user is successfully redirected to the dashboard.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Login Failure with Incorrect Email</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Click the 'Login' button.</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>An error message is displayed indicating an empty password field is required.</t>
-        </is>
-      </c>
+          <t>Navigate to the login page.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Validate Incorrect Email and Password Combination</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Navigate to the login page.</t>
+          <t>Enter an incorrect email address into the 'Email' field.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -598,7 +598,7 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Enter an invalid email address and password.</t>
+          <t>Enter a valid password into the 'Password' field.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -612,14 +612,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>An error message is displayed indicating the entered credentials are incorrect.</t>
+          <t>An error message is displayed informing the user that the email or password is incorrect.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Verify Successful Login</t>
+          <t>Login Failure with Incorrect Password</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -633,7 +633,7 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Enter a valid email address and password.</t>
+          <t>Enter a valid email address into the 'Email' field.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -642,33 +642,33 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Enter an incorrect password into the 'Password' field.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>Click the 'Login' button.</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>The user is redirected to the designated dashboard page.</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Test Login Rate Limiting</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>An error message is displayed informing the user that the email or password is incorrect.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Login Attempt Limit Exceeded</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Navigate to the login page.</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Enter invalid credentials and attempt to login 5 times consecutively.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -677,12 +677,21 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Observe the response after the 5th attempt.</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>An error message is displayed informing the user of a temporary login lockout.</t>
+          <t>Attempt to login with incorrect credentials 5 times within an hour.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Attempt to login again with incorrect credentials.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>An error message is displayed informing the user that they have exceeded the login attempt limit. The message should also provide an estimated time for the restriction to be lifted.</t>
         </is>
       </c>
     </row>

</xml_diff>